<commit_message>
Update file Excel cassa and image Rendiconto cassa
</commit_message>
<xml_diff>
--- a/ets/rendiconti2020/rendiconti-excel-word/rendiconto-per-cassa-modello-excel.xlsx
+++ b/ets/rendiconti2020/rendiconti-excel-word/rendiconto-per-cassa-modello-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.mercurio\Documents\GitHub\Italia\ets\rendiconti2020\rendiconti-excel-word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EB2966-68E0-FC4F-923B-D7A23ADDDDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D186C053-E43C-42C4-8362-6AAC54A43C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23700" windowHeight="14560" xr2:uid="{FF94FDBB-7E1C-4349-A12A-5CA933A991FE}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF94FDBB-7E1C-4349-A12A-5CA933A991FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -275,9 +279,6 @@
   </si>
   <si>
     <t>TOTALE ENTRATE DELLA GESTIONE</t>
-  </si>
-  <si>
-    <t>ASSOCIAZIONE XX - RENDICONTO PER CASSA ANNO 2021</t>
   </si>
   <si>
     <t xml:space="preserve">Con Banana Contabilità Plus è ancora più semplice: </t>
@@ -319,13 +320,16 @@
       <t>Cassa e Banca dell'anno precedente + Avanzo/Disavanzo corrente = Cassa e Banca corrente</t>
     </r>
   </si>
+  <si>
+    <t>ASSOCIAZIONE XX - RENDICONTO PER CASSA ANNO 2024</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -427,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -445,34 +449,31 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -491,9 +492,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -531,7 +532,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -637,7 +638,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -779,7 +780,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -794,75 +795,75 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" customWidth="1"/>
-    <col min="5" max="5" width="52.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6796875" customWidth="1"/>
+    <col min="2" max="2" width="14.31640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6796875" customWidth="1"/>
+    <col min="4" max="4" width="6.1796875" customWidth="1"/>
+    <col min="5" max="5" width="52.31640625" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14.6796875" customWidth="1"/>
+    <col min="8" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="21" x14ac:dyDescent="1">
+      <c r="A2" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.8">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="27">
-        <v>44561</v>
-      </c>
-      <c r="C8" s="27">
-        <v>44196</v>
+      <c r="B8" s="18">
+        <v>45657</v>
+      </c>
+      <c r="C8" s="18">
+        <v>45291</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="18">
         <f>B8</f>
-        <v>44561</v>
-      </c>
-      <c r="G8" s="27">
+        <v>45657</v>
+      </c>
+      <c r="G8" s="18">
         <f>C8</f>
-        <v>44196</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -870,194 +871,194 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="16">
-        <v>0</v>
-      </c>
-      <c r="C10" s="16">
+      <c r="B10" s="14">
+        <v>0</v>
+      </c>
+      <c r="C10" s="14">
         <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="16">
-        <v>0</v>
-      </c>
-      <c r="G10" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F10" s="14">
+        <v>0</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="16">
-        <v>0</v>
-      </c>
-      <c r="C11" s="16">
+      <c r="B11" s="14">
+        <v>0</v>
+      </c>
+      <c r="C11" s="14">
         <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="16">
-        <v>0</v>
-      </c>
-      <c r="G11" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F11" s="14">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="16">
-        <v>0</v>
-      </c>
-      <c r="C12" s="16">
+      <c r="B12" s="14">
+        <v>0</v>
+      </c>
+      <c r="C12" s="14">
         <v>0</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="16">
-        <v>0</v>
-      </c>
-      <c r="G12" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F12" s="14">
+        <v>0</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="16">
-        <v>0</v>
-      </c>
-      <c r="C13" s="16">
+      <c r="B13" s="14">
+        <v>0</v>
+      </c>
+      <c r="C13" s="14">
         <v>0</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="16">
-        <v>0</v>
-      </c>
-      <c r="G13" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F13" s="14">
+        <v>0</v>
+      </c>
+      <c r="G13" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="16">
-        <v>0</v>
-      </c>
-      <c r="C14" s="16">
+      <c r="B14" s="14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="16">
-        <v>0</v>
-      </c>
-      <c r="G14" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F14" s="14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E15" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="16">
-        <v>0</v>
-      </c>
-      <c r="G15" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F15" s="14">
+        <v>0</v>
+      </c>
+      <c r="G15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E16" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="16">
-        <v>0</v>
-      </c>
-      <c r="G16" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F16" s="14">
+        <v>0</v>
+      </c>
+      <c r="G16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="16">
-        <v>0</v>
-      </c>
-      <c r="G17" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F17" s="14">
+        <v>0</v>
+      </c>
+      <c r="G17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E18" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="16">
-        <v>0</v>
-      </c>
-      <c r="G18" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F18" s="14">
+        <v>0</v>
+      </c>
+      <c r="G18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E19" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="16">
-        <v>0</v>
-      </c>
-      <c r="G19" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+      <c r="F19" s="14">
+        <v>0</v>
+      </c>
+      <c r="G19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="12">
         <f>SUM(B10:B14)</f>
         <v>0</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="12">
         <f>SUM(C10:C14)</f>
         <v>0</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="12">
         <f>SUM(F10:F19)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="12">
         <f>SUM(G10:G19)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A21" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="10">
         <f>F20-B20</f>
         <v>0</v>
@@ -1067,14 +1068,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A23" s="4" t="s">
         <v>26</v>
       </c>
@@ -1082,150 +1083,150 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="16">
-        <v>0</v>
-      </c>
-      <c r="C24" s="16">
+      <c r="B24" s="14">
+        <v>0</v>
+      </c>
+      <c r="C24" s="14">
         <v>0</v>
       </c>
       <c r="E24" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="16">
-        <v>0</v>
-      </c>
-      <c r="G24" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F24" s="14">
+        <v>0</v>
+      </c>
+      <c r="G24" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="16">
-        <v>0</v>
-      </c>
-      <c r="C25" s="16">
+      <c r="B25" s="14">
+        <v>0</v>
+      </c>
+      <c r="C25" s="14">
         <v>0</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="16">
-        <v>0</v>
-      </c>
-      <c r="G25" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F25" s="14">
+        <v>0</v>
+      </c>
+      <c r="G25" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="16">
-        <v>0</v>
-      </c>
-      <c r="C26" s="16">
+      <c r="B26" s="14">
+        <v>0</v>
+      </c>
+      <c r="C26" s="14">
         <v>0</v>
       </c>
       <c r="E26" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="16">
-        <v>0</v>
-      </c>
-      <c r="G26" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F26" s="14">
+        <v>0</v>
+      </c>
+      <c r="G26" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="16">
-        <v>0</v>
-      </c>
-      <c r="C27" s="16">
+      <c r="B27" s="14">
+        <v>0</v>
+      </c>
+      <c r="C27" s="14">
         <v>0</v>
       </c>
       <c r="E27" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="16">
-        <v>0</v>
-      </c>
-      <c r="G27" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F27" s="14">
+        <v>0</v>
+      </c>
+      <c r="G27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="16">
-        <v>0</v>
-      </c>
-      <c r="C28" s="16">
+      <c r="B28" s="14">
+        <v>0</v>
+      </c>
+      <c r="C28" s="14">
         <v>0</v>
       </c>
       <c r="E28" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="16">
-        <v>0</v>
-      </c>
-      <c r="G28" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F28" s="14">
+        <v>0</v>
+      </c>
+      <c r="G28" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E29" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="16">
-        <v>0</v>
-      </c>
-      <c r="G29" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
+      <c r="F29" s="14">
+        <v>0</v>
+      </c>
+      <c r="G29" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A30" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="12">
         <f>SUM(B24:B28)</f>
         <v>0</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="12">
         <f>SUM(C24:C28)</f>
         <v>0</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="12">
         <f>SUM(F24:F29)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="12">
         <f>SUM(G24:G29)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="22" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A31" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
       <c r="F31" s="10">
         <f>F30-B30</f>
         <v>0</v>
@@ -1235,14 +1236,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
@@ -1250,99 +1251,99 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="16">
-        <v>0</v>
-      </c>
-      <c r="C34" s="16">
+      <c r="B34" s="14">
+        <v>0</v>
+      </c>
+      <c r="C34" s="14">
         <v>0</v>
       </c>
       <c r="E34" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="16">
-        <v>0</v>
-      </c>
-      <c r="G34" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F34" s="14">
+        <v>0</v>
+      </c>
+      <c r="G34" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="16">
-        <v>0</v>
-      </c>
-      <c r="C35" s="16">
+      <c r="B35" s="14">
+        <v>0</v>
+      </c>
+      <c r="C35" s="14">
         <v>0</v>
       </c>
       <c r="E35" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="16">
-        <v>0</v>
-      </c>
-      <c r="G35" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F35" s="14">
+        <v>0</v>
+      </c>
+      <c r="G35" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="16">
-        <v>0</v>
-      </c>
-      <c r="C36" s="16">
+      <c r="B36" s="14">
+        <v>0</v>
+      </c>
+      <c r="C36" s="14">
         <v>0</v>
       </c>
       <c r="E36" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="16">
-        <v>0</v>
-      </c>
-      <c r="G36" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
+      <c r="F36" s="14">
+        <v>0</v>
+      </c>
+      <c r="G36" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A37" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="12">
         <f>SUM(B34:B36)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="13">
+      <c r="C37" s="12">
         <f>SUM(C34:C36)</f>
         <v>0</v>
       </c>
       <c r="D37" s="4"/>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="12">
         <f>SUM(F34:F36)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G37" s="12">
         <f>SUM(G34:G36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A38" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="10">
         <f>F37-B37</f>
         <v>0</v>
@@ -1352,14 +1353,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1367,139 +1368,139 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="16">
-        <v>0</v>
-      </c>
-      <c r="C41" s="16">
+      <c r="B41" s="14">
+        <v>0</v>
+      </c>
+      <c r="C41" s="14">
         <v>0</v>
       </c>
       <c r="E41" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="16">
-        <v>0</v>
-      </c>
-      <c r="G41" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F41" s="14">
+        <v>0</v>
+      </c>
+      <c r="G41" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="16">
-        <v>0</v>
-      </c>
-      <c r="C42" s="16">
+      <c r="B42" s="14">
+        <v>0</v>
+      </c>
+      <c r="C42" s="14">
         <v>0</v>
       </c>
       <c r="E42" t="s">
         <v>49</v>
       </c>
-      <c r="F42" s="16">
-        <v>0</v>
-      </c>
-      <c r="G42" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F42" s="14">
+        <v>0</v>
+      </c>
+      <c r="G42" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="16">
-        <v>0</v>
-      </c>
-      <c r="C43" s="16">
+      <c r="B43" s="14">
+        <v>0</v>
+      </c>
+      <c r="C43" s="14">
         <v>0</v>
       </c>
       <c r="E43" t="s">
         <v>51</v>
       </c>
-      <c r="F43" s="16">
-        <v>0</v>
-      </c>
-      <c r="G43" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F43" s="14">
+        <v>0</v>
+      </c>
+      <c r="G43" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="16">
-        <v>0</v>
-      </c>
-      <c r="C44" s="16">
+      <c r="B44" s="14">
+        <v>0</v>
+      </c>
+      <c r="C44" s="14">
         <v>0</v>
       </c>
       <c r="E44" t="s">
         <v>53</v>
       </c>
-      <c r="F44" s="16">
-        <v>0</v>
-      </c>
-      <c r="G44" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F44" s="14">
+        <v>0</v>
+      </c>
+      <c r="G44" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="16">
-        <v>0</v>
-      </c>
-      <c r="C45" s="16">
+      <c r="B45" s="14">
+        <v>0</v>
+      </c>
+      <c r="C45" s="14">
         <v>0</v>
       </c>
       <c r="E45" t="s">
         <v>55</v>
       </c>
-      <c r="F45" s="16">
-        <v>0</v>
-      </c>
-      <c r="G45" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
+      <c r="F45" s="14">
+        <v>0</v>
+      </c>
+      <c r="G45" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A46" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B46" s="12">
         <f>SUM(B41:B45)</f>
         <v>0</v>
       </c>
-      <c r="C46" s="13">
+      <c r="C46" s="12">
         <f>SUM(C41:C45)</f>
         <v>0</v>
       </c>
       <c r="D46" s="4"/>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="13">
+      <c r="F46" s="12">
         <f>SUM(F41:F45)</f>
         <v>0</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="12">
         <f>SUM(G41:G45)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="22" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A47" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
       <c r="F47" s="10">
         <f>F46-B46</f>
         <v>0</v>
@@ -1509,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A49" s="4" t="s">
         <v>57</v>
       </c>
@@ -1517,140 +1518,140 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="16">
-        <v>0</v>
-      </c>
-      <c r="C50" s="16">
+      <c r="B50" s="14">
+        <v>0</v>
+      </c>
+      <c r="C50" s="14">
         <v>0</v>
       </c>
       <c r="E50" t="s">
         <v>59</v>
       </c>
-      <c r="F50" s="16">
-        <v>0</v>
-      </c>
-      <c r="G50" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F50" s="14">
+        <v>0</v>
+      </c>
+      <c r="G50" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A51" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="16">
-        <v>0</v>
-      </c>
-      <c r="C51" s="16">
+      <c r="B51" s="14">
+        <v>0</v>
+      </c>
+      <c r="C51" s="14">
         <v>0</v>
       </c>
       <c r="E51" t="s">
         <v>60</v>
       </c>
-      <c r="F51" s="16">
-        <v>0</v>
-      </c>
-      <c r="G51" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F51" s="14">
+        <v>0</v>
+      </c>
+      <c r="G51" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A52" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="16">
-        <v>0</v>
-      </c>
-      <c r="C52" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B52" s="14">
+        <v>0</v>
+      </c>
+      <c r="C52" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A53" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="16">
-        <v>0</v>
-      </c>
-      <c r="C53" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B53" s="14">
+        <v>0</v>
+      </c>
+      <c r="C53" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A54" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="16">
-        <v>0</v>
-      </c>
-      <c r="C54" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="12" t="s">
+      <c r="B54" s="14">
+        <v>0</v>
+      </c>
+      <c r="C54" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A55" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="13">
+      <c r="B55" s="12">
         <f>SUM(B50:B54)</f>
         <v>0</v>
       </c>
-      <c r="C55" s="13">
+      <c r="C55" s="12">
         <f>SUM(C50:C54)</f>
         <v>0</v>
       </c>
       <c r="D55" s="4"/>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="13">
+      <c r="F55" s="12">
         <f>SUM(F50:F51)</f>
         <v>0</v>
       </c>
-      <c r="G55" s="13">
+      <c r="G55" s="12">
         <f>SUM(G50:G51)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A56" s="7"/>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A57" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="13">
+      <c r="B57" s="12">
         <f>B20+B30+B37+B46+B55</f>
         <v>0</v>
       </c>
-      <c r="C57" s="13">
+      <c r="C57" s="12">
         <f>C20+C30+C37+C46+C55</f>
         <v>0</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F57" s="13">
+      <c r="F57" s="12">
         <f>F20+F30+F37+F46+F55</f>
         <v>0</v>
       </c>
-      <c r="G57" s="13">
+      <c r="G57" s="12">
         <f>G20+G30+G37+G46+G55</f>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="22" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A58" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="22"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
       <c r="F58" s="10">
         <f>F57-B57</f>
         <v>0</v>
@@ -1660,29 +1661,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="22" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A59" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="15">
-        <v>0</v>
-      </c>
-      <c r="G59" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="22" t="s">
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="13">
+        <v>0</v>
+      </c>
+      <c r="G59" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A60" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="22"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
       <c r="F60" s="10">
         <f>F58-F59</f>
         <v>0</v>
@@ -1692,171 +1693,171 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="32" x14ac:dyDescent="0.8">
       <c r="A63" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B63" s="27">
+      <c r="B63" s="18">
         <f>B8</f>
-        <v>44561</v>
-      </c>
-      <c r="C63" s="27">
+        <v>45657</v>
+      </c>
+      <c r="C63" s="18">
         <f>C8</f>
-        <v>44196</v>
+        <v>45291</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F63" s="27">
+      <c r="F63" s="18">
         <f>B8</f>
-        <v>44561</v>
-      </c>
-      <c r="G63" s="27">
+        <v>45657</v>
+      </c>
+      <c r="G63" s="18">
         <f>C8</f>
-        <v>44196</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A64" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="16">
-        <v>0</v>
-      </c>
-      <c r="C64" s="16">
+      <c r="B64" s="14">
+        <v>0</v>
+      </c>
+      <c r="C64" s="14">
         <v>0</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F64" s="16">
-        <v>0</v>
-      </c>
-      <c r="G64" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="F64" s="14">
+        <v>0</v>
+      </c>
+      <c r="G64" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A65" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="16">
-        <v>0</v>
-      </c>
-      <c r="C65" s="16">
+      <c r="B65" s="14">
+        <v>0</v>
+      </c>
+      <c r="C65" s="14">
         <v>0</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F65" s="16">
-        <v>0</v>
-      </c>
-      <c r="G65" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F65" s="14">
+        <v>0</v>
+      </c>
+      <c r="G65" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A66" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="16">
-        <v>0</v>
-      </c>
-      <c r="C66" s="16">
+      <c r="B66" s="14">
+        <v>0</v>
+      </c>
+      <c r="C66" s="14">
         <v>0</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F66" s="16">
-        <v>0</v>
-      </c>
-      <c r="G66" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="F66" s="14">
+        <v>0</v>
+      </c>
+      <c r="G66" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A67" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="16">
-        <v>0</v>
-      </c>
-      <c r="C67" s="16">
+      <c r="B67" s="14">
+        <v>0</v>
+      </c>
+      <c r="C67" s="14">
         <v>0</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F67" s="16">
-        <v>0</v>
-      </c>
-      <c r="G67" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="12" t="s">
+      <c r="F67" s="14">
+        <v>0</v>
+      </c>
+      <c r="G67" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A68" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="13">
+      <c r="B68" s="12">
         <f>SUM(B64:B67)</f>
         <v>0</v>
       </c>
-      <c r="C68" s="13">
+      <c r="C68" s="12">
         <f>SUM(C64:C67)</f>
         <v>0</v>
       </c>
       <c r="D68" s="4"/>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F68" s="13">
+      <c r="F68" s="12">
         <f>SUM(F64:F67)</f>
         <v>0</v>
       </c>
-      <c r="G68" s="13">
+      <c r="G68" s="12">
         <f>SUM(G64:G67)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="22" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A69" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="15">
-        <v>0</v>
-      </c>
-      <c r="G69" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="22" t="s">
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="13">
+        <v>0</v>
+      </c>
+      <c r="G69" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A70" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="22"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
       <c r="F70" s="10">
         <f>F68-B68</f>
         <v>0</v>
@@ -1866,41 +1867,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A72" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="26"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="26"/>
-      <c r="E73" s="26"/>
-      <c r="F73" s="28">
+    <row r="73" spans="1:7" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.8">
+      <c r="A73" s="23"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="19">
         <f>B8</f>
-        <v>44561</v>
-      </c>
-      <c r="G73" s="28">
+        <v>45657</v>
+      </c>
+      <c r="G73" s="19">
         <f>C8</f>
-        <v>44196</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="22" t="s">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A74" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B74" s="22"/>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
       <c r="F74" s="10">
         <f>F60</f>
         <v>0</v>
@@ -1910,14 +1911,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="22" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A75" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="22"/>
-      <c r="C75" s="22"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
       <c r="F75" s="10">
         <f>F70</f>
         <v>0</v>
@@ -1927,14 +1928,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="22" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A76" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="22"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="22"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
       <c r="F76" s="10">
         <f>F74+F75-F69</f>
         <v>0</v>
@@ -1944,213 +1945,213 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A77" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="23" t="s">
+    <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.8">
+      <c r="A79" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B79" s="23"/>
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
-      <c r="E79" s="23"/>
-      <c r="F79" s="28">
+      <c r="B79" s="25"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="19">
         <f>B8</f>
-        <v>44561</v>
-      </c>
-      <c r="G79" s="28">
+        <v>45657</v>
+      </c>
+      <c r="G79" s="19">
         <f>C8</f>
-        <v>44196</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="24" t="s">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A80" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="16">
-        <v>0</v>
-      </c>
-      <c r="G80" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" s="24" t="s">
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="14">
+        <v>0</v>
+      </c>
+      <c r="G80" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A81" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="16">
-        <v>0</v>
-      </c>
-      <c r="G81" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="14">
+        <v>0</v>
+      </c>
+      <c r="G81" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="16" x14ac:dyDescent="0.8">
       <c r="A84" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B84" s="28">
+      <c r="B84" s="19">
         <f>B8</f>
-        <v>44561</v>
-      </c>
-      <c r="C84" s="28">
+        <v>45657</v>
+      </c>
+      <c r="C84" s="19">
         <f>C8</f>
-        <v>44196</v>
+        <v>45291</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F84" s="28">
+      <c r="F84" s="19">
         <f>B8</f>
-        <v>44561</v>
-      </c>
-      <c r="G84" s="28">
+        <v>45657</v>
+      </c>
+      <c r="G84" s="19">
         <f>C8</f>
-        <v>44196</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A85" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="15">
-        <v>0</v>
-      </c>
-      <c r="C85" s="15">
+      <c r="B85" s="13">
+        <v>0</v>
+      </c>
+      <c r="C85" s="13">
         <v>0</v>
       </c>
       <c r="E85" t="s">
         <v>3</v>
       </c>
-      <c r="F85" s="15">
-        <v>0</v>
-      </c>
-      <c r="G85" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F85" s="13">
+        <v>0</v>
+      </c>
+      <c r="G85" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A86" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="15">
-        <v>0</v>
-      </c>
-      <c r="C86" s="15">
+      <c r="B86" s="13">
+        <v>0</v>
+      </c>
+      <c r="C86" s="13">
         <v>0</v>
       </c>
       <c r="E86" t="s">
         <v>4</v>
       </c>
-      <c r="F86" s="15">
-        <v>0</v>
-      </c>
-      <c r="G86" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="12" t="s">
+      <c r="F86" s="13">
+        <v>0</v>
+      </c>
+      <c r="G86" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A87" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="13">
+      <c r="B87" s="12">
         <f>SUM(B85:B86)</f>
         <v>0</v>
       </c>
-      <c r="C87" s="13">
+      <c r="C87" s="12">
         <f>SUM(C85:C86)</f>
         <v>0</v>
       </c>
       <c r="D87" s="4"/>
-      <c r="E87" s="12" t="s">
+      <c r="E87" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F87" s="13">
+      <c r="F87" s="12">
         <f>SUM(F85:F86)</f>
         <v>0</v>
       </c>
-      <c r="G87" s="13">
+      <c r="G87" s="12">
         <f>SUM(G85:G86)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.75">
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="92" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A92" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B92" s="5"/>
     </row>
-    <row r="93" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="17" t="s">
+    <row r="93" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A93" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B93" s="16">
+        <f>G80+G81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A94" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B93" s="18">
-        <f>G80+G81</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="17" t="s">
+      <c r="B94" s="16">
+        <f>F76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A95" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B94" s="18">
-        <f>F76</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="17" t="s">
+      <c r="B95" s="16">
+        <f>F80+F81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A96" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B95" s="18">
-        <f>F80+F81</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B96" s="21" t="str">
+      <c r="B96" s="24" t="str">
         <f>IF((B93+B94)=B95,"Quadratura OK","Errore quadratura")</f>
         <v>Quadratura OK</v>
       </c>
-      <c r="C96" s="21"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="20"/>
-      <c r="G96" s="20"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11"/>
+      <c r="C96" s="24"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="15"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A98" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="A76:E76"/>
+    <mergeCell ref="A79:E79"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A81:E81"/>
     <mergeCell ref="A74:E74"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A21:E21"/>
@@ -2163,12 +2164,6 @@
     <mergeCell ref="A69:E69"/>
     <mergeCell ref="A70:E70"/>
     <mergeCell ref="A73:E73"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="A75:E75"/>
-    <mergeCell ref="A76:E76"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A81:E81"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiornato descrizione Banana file Excel ETS
</commit_message>
<xml_diff>
--- a/ets/rendiconti2020/rendiconti-excel-word/rendiconto-per-cassa-modello-excel.xlsx
+++ b/ets/rendiconti2020/rendiconti-excel-word/rendiconto-per-cassa-modello-excel.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan/GitHub/BananaAccounting/Italia/ets/rendiconti2020/rendiconti-excel-word/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.mercurio\Documents\GitHub\Italia\ets\rendiconti2020\rendiconti-excel-word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{85BE384D-E01B-9E42-9E6E-A6C903DC0B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{650A5855-E693-4845-BF11-0FA4B2CD4FB9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E84D28D-9E7D-47FC-A5E1-FC4FB1F37430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5800" yWindow="1680" windowWidth="29380" windowHeight="26660" xr2:uid="{FF94FDBB-7E1C-4349-A12A-5CA933A991FE}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF94FDBB-7E1C-4349-A12A-5CA933A991FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Foglio1!$A$7:$G$133</definedName>
     <definedName name="FormatoStampa">Foglio1!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Foglio1!$A$7:$G$128</definedName>
     <definedName name="ZonaInserimento">Foglio1!$B$14:$C$18,Foglio1!$B$28:$C$32,Foglio1!$B$38:$C$40,Foglio1!$B$45:$C$49,Foglio1!$B$54:$C$58,Foglio1!$B$68:$C$71,Foglio1!$F$14:$G$23,Foglio1!$F$28:$G$33,Foglio1!$F$38:$G$40,Foglio1!$F$45:$G$49,Foglio1!$F$54:$G$55,Foglio1!$F$63:$G$63,Foglio1!$F$68:$G$71,Foglio1!$F$73:$G$73,Foglio1!$F$84:$G$85,Foglio1!$F$89:$G$90,Foglio1!$B$89:$C$90</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="116">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -361,9 +361,6 @@
     <t>Note / Personalizzazioni</t>
   </si>
   <si>
-    <t>Il rendiconto per cassa e gli altri rendiconti si ottengono in automatico partendo dalle registrazioni contabili.</t>
-  </si>
-  <si>
     <t>Facile da usare (Simile a Excel) e gratuito fino a 70 registrazioni.</t>
   </si>
   <si>
@@ -376,7 +373,42 @@
     <t>Si</t>
   </si>
   <si>
-    <t>Con Banana Contabilità Plus è più veloce e semplice: </t>
+    <t>Ogni ente è obbligato a mantenere una raccolta completa e ordinata dei documenti (fatture, ricevute e altri documenti), conservandoli in modo sistematico e facilmente reperibile.</t>
+  </si>
+  <si>
+    <t>Una raccolta ordinata dei documenti non è però sufficiente, in molti casi è utile fare anche la registrazione cronologica e sistematica dei movimenti.</t>
+  </si>
+  <si>
+    <t>Banana Contabilità</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Con Banana Contabilità questo passo</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> è molto semplice e veloce:</t>
+    </r>
+  </si>
+  <si>
+    <t>Ti permette di fare la registrazione cronologica e sistematica dei movimenti (collegandoli ai documenti), una prima nota.</t>
+  </si>
+  <si>
+    <t>In questo modo potrai anche ottenere in automatico il Rendiconto per cassa e altri rendiconti.</t>
   </si>
 </sst>
 </file>
@@ -387,7 +419,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,6 +516,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -518,7 +562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -565,20 +609,25 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -622,7 +671,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -918,30 +967,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5901BA8-36CC-4DBE-B6A9-97354061FBEE}">
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" customWidth="1"/>
-    <col min="5" max="5" width="52.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6796875" customWidth="1"/>
+    <col min="2" max="2" width="16.6796875" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="4" max="4" width="6.1796875" customWidth="1"/>
+    <col min="5" max="5" width="52.31640625" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14.6796875" customWidth="1"/>
+    <col min="8" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" s="24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -949,7 +998,7 @@
         <v>46022</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -957,24 +1006,24 @@
         <v>45657</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>96</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="21" x14ac:dyDescent="1">
+      <c r="A7" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-    </row>
-    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+    </row>
+    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="1">
       <c r="A8" s="3" t="s">
         <v>85</v>
       </c>
@@ -983,19 +1032,19 @@
         <v>46022</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="1">
       <c r="A9" t="s">
         <v>104</v>
       </c>
       <c r="B9" s="21"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B10" s="19"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B11" s="19"/>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.8">
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
@@ -1019,7 +1068,7 @@
         <v>45657</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1029,7 +1078,7 @@
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1049,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1069,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1089,7 +1138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1109,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1129,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E19" t="s">
         <v>20</v>
       </c>
@@ -1140,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E20" t="s">
         <v>21</v>
       </c>
@@ -1151,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E21" t="s">
         <v>22</v>
       </c>
@@ -1162,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E22" t="s">
         <v>23</v>
       </c>
@@ -1173,7 +1222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E23" t="s">
         <v>24</v>
       </c>
@@ -1184,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A24" s="11" t="s">
         <v>5</v>
       </c>
@@ -1209,14 +1258,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="29" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A25" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
       <c r="F25" s="10">
         <f>F24-B24</f>
         <v>0</v>
@@ -1226,14 +1275,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
@@ -1241,7 +1290,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1261,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1281,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1301,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1321,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1341,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
       <c r="E33" t="s">
         <v>33</v>
       </c>
@@ -1352,7 +1401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A34" s="11" t="s">
         <v>5</v>
       </c>
@@ -1377,14 +1426,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A35" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
       <c r="F35" s="10">
         <f>F34-B34</f>
         <v>0</v>
@@ -1394,14 +1443,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A37" s="4" t="s">
         <v>35</v>
       </c>
@@ -1409,7 +1458,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1429,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1449,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1469,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A41" s="11" t="s">
         <v>5</v>
       </c>
@@ -1494,14 +1543,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="29" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A42" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
       <c r="F42" s="10">
         <f>F41-B41</f>
         <v>0</v>
@@ -1511,14 +1560,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A44" s="4" t="s">
         <v>44</v>
       </c>
@@ -1526,7 +1575,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1546,7 +1595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -1566,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1586,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1606,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -1626,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A50" s="11" t="s">
         <v>5</v>
       </c>
@@ -1651,14 +1700,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="29" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A51" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
       <c r="F51" s="10">
         <f>F50-B50</f>
         <v>0</v>
@@ -1668,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A53" s="4" t="s">
         <v>57</v>
       </c>
@@ -1676,7 +1725,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -1696,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -1716,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -1727,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -1738,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -1749,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A59" s="11" t="s">
         <v>5</v>
       </c>
@@ -1774,11 +1823,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A60" s="7"/>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A61" s="4" t="s">
         <v>61</v>
       </c>
@@ -1802,14 +1851,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="29" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A62" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="29"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
       <c r="F62" s="10">
         <f>F61-B61</f>
         <v>0</v>
@@ -1819,14 +1868,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="29" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A63" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="29"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
       <c r="F63" s="10">
         <v>0</v>
       </c>
@@ -1834,14 +1883,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="29" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A64" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="29"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="29"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
       <c r="F64" s="10">
         <f>F62-F63</f>
         <v>0</v>
@@ -1851,19 +1900,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A66" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="32" x14ac:dyDescent="0.8">
       <c r="A67" s="9" t="s">
         <v>65</v>
       </c>
@@ -1888,7 +1937,7 @@
         <v>45657</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A68" s="8" t="s">
         <v>67</v>
       </c>
@@ -1908,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A69" s="8" t="s">
         <v>69</v>
       </c>
@@ -1928,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A70" s="8" t="s">
         <v>71</v>
       </c>
@@ -1948,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A71" s="8" t="s">
         <v>73</v>
       </c>
@@ -1968,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A72" s="11" t="s">
         <v>5</v>
       </c>
@@ -1993,14 +2042,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="29" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A73" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B73" s="29"/>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
-      <c r="E73" s="29"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
       <c r="F73" s="10">
         <v>0</v>
       </c>
@@ -2008,14 +2057,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="29" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A74" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B74" s="29"/>
-      <c r="C74" s="29"/>
-      <c r="D74" s="29"/>
-      <c r="E74" s="29"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
       <c r="F74" s="10">
         <f>F72-B72</f>
         <v>0</v>
@@ -2025,24 +2074,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A76" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="33"/>
-      <c r="B77" s="33"/>
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="33"/>
+    <row r="77" spans="1:7" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.8">
+      <c r="A77" s="31"/>
+      <c r="B77" s="31"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
       <c r="F77" s="17">
         <f>B12</f>
         <v>46022</v>
@@ -2052,14 +2101,14 @@
         <v>45657</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="29" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A78" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B78" s="29"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
+      <c r="B78" s="28"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="28"/>
       <c r="F78" s="10">
         <f>F64</f>
         <v>0</v>
@@ -2069,14 +2118,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="29" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A79" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B79" s="29"/>
-      <c r="C79" s="29"/>
-      <c r="D79" s="29"/>
-      <c r="E79" s="29"/>
+      <c r="B79" s="28"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="28"/>
       <c r="F79" s="10">
         <f>F74</f>
         <v>0</v>
@@ -2086,14 +2135,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="29" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A80" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B80" s="29"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="29"/>
-      <c r="E80" s="29"/>
+      <c r="B80" s="28"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="28"/>
       <c r="F80" s="10">
         <f>F78+F79-F73</f>
         <v>0</v>
@@ -2103,19 +2152,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A81" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="30" t="s">
+    <row r="83" spans="1:9" ht="16" x14ac:dyDescent="0.8">
+      <c r="A83" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B83" s="30"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="30"/>
-      <c r="E83" s="30"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="33"/>
       <c r="F83" s="17">
         <f>B12</f>
         <v>46022</v>
@@ -2125,14 +2174,14 @@
         <v>45657</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="31" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A84" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="B84" s="31"/>
-      <c r="C84" s="31"/>
-      <c r="D84" s="31"/>
-      <c r="E84" s="31"/>
+      <c r="B84" s="30"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="30"/>
       <c r="F84" s="20">
         <v>0</v>
       </c>
@@ -2140,14 +2189,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="31" t="s">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A85" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="B85" s="31"/>
-      <c r="C85" s="31"/>
-      <c r="D85" s="31"/>
-      <c r="E85" s="31"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
       <c r="F85" s="20">
         <v>0</v>
       </c>
@@ -2155,7 +2204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="16" x14ac:dyDescent="0.8">
       <c r="A88" s="6" t="s">
         <v>1</v>
       </c>
@@ -2179,7 +2228,7 @@
         <v>45657</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -2199,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A90" t="s">
         <v>4</v>
       </c>
@@ -2219,7 +2268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A91" s="11" t="s">
         <v>5</v>
       </c>
@@ -2244,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A92" s="11"/>
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
@@ -2253,7 +2302,7 @@
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A93" s="11"/>
       <c r="B93" s="12"/>
       <c r="C93" s="12"/>
@@ -2262,19 +2311,19 @@
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.75">
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
     </row>
-    <row r="98" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A98" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B98" s="5"/>
     </row>
-    <row r="99" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A99" s="13" t="s">
         <v>81</v>
       </c>
@@ -2283,7 +2332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A100" s="13" t="s">
         <v>82</v>
       </c>
@@ -2292,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A101" s="5" t="s">
         <v>98</v>
       </c>
@@ -2301,7 +2350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A102" s="13" t="s">
         <v>83</v>
       </c>
@@ -2310,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A103" s="5" t="s">
         <v>97</v>
       </c>
@@ -2319,141 +2368,175 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A104" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B104" s="28" t="str">
+      <c r="B104" s="32" t="str">
         <f>IF(B103=0,"Quadratura OK","Errore quadratura")</f>
         <v>Quadratura OK</v>
       </c>
-      <c r="C104" s="28"/>
+      <c r="C104" s="32"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
       <c r="F104" s="13"/>
       <c r="G104" s="13"/>
     </row>
-    <row r="107" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="16" x14ac:dyDescent="0.8">
       <c r="A107" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B107" s="13"/>
     </row>
-    <row r="108" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="16" x14ac:dyDescent="0.8">
       <c r="A108" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B108" s="13"/>
     </row>
-    <row r="109" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="16" x14ac:dyDescent="0.8">
       <c r="A109" s="13" t="s">
         <v>102</v>
       </c>
       <c r="B109" s="13"/>
     </row>
-    <row r="110" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="16" x14ac:dyDescent="0.8">
       <c r="A110" s="13" t="s">
         <v>103</v>
       </c>
       <c r="B110" s="13"/>
     </row>
-    <row r="111" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" ht="16" x14ac:dyDescent="0.8">
       <c r="B111" s="13"/>
     </row>
-    <row r="112" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" ht="16" x14ac:dyDescent="0.8">
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
     </row>
-    <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.8">
       <c r="A113" s="13" t="s">
         <v>94</v>
       </c>
       <c r="B113" s="13"/>
     </row>
-    <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.8">
       <c r="A114" s="13" t="s">
         <v>101</v>
       </c>
       <c r="B114" s="13"/>
     </row>
-    <row r="115" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" ht="16" x14ac:dyDescent="0.8">
       <c r="A115" s="27" t="s">
         <v>93</v>
       </c>
       <c r="B115" s="13"/>
     </row>
-    <row r="116" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" ht="16" x14ac:dyDescent="0.8">
       <c r="A116" s="26" t="s">
         <v>100</v>
       </c>
       <c r="B116" s="13"/>
     </row>
-    <row r="117" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" ht="16" x14ac:dyDescent="0.8">
       <c r="A117" s="26"/>
       <c r="B117" s="13"/>
     </row>
-    <row r="118" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="5" t="s">
+    <row r="118" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A118" s="26"/>
+      <c r="B118" s="13"/>
+    </row>
+    <row r="119" spans="1:2" s="23" customFormat="1" ht="16" x14ac:dyDescent="0.8">
+      <c r="A119" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B119" s="38"/>
+    </row>
+    <row r="120" spans="1:2" s="36" customFormat="1" ht="16" x14ac:dyDescent="0.8">
+      <c r="A120" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B120" s="35"/>
+    </row>
+    <row r="121" spans="1:2" s="36" customFormat="1" ht="16" x14ac:dyDescent="0.8">
+      <c r="A121" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="B118" s="13"/>
-    </row>
-    <row r="119" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="13" t="s">
+      <c r="B121" s="35"/>
+    </row>
+    <row r="122" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A122" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B122" s="13"/>
+    </row>
+    <row r="123" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A123" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B123" s="13"/>
+    </row>
+    <row r="124" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A124" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B124" s="13"/>
+    </row>
+    <row r="125" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A125" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B119" s="13"/>
-    </row>
-    <row r="120" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="13" t="s">
+      <c r="B125" s="13"/>
+    </row>
+    <row r="126" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A126" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B126" s="13"/>
+    </row>
+    <row r="127" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A127" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B127" s="13"/>
+    </row>
+    <row r="128" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A128" s="13"/>
+      <c r="B128" s="13"/>
+    </row>
+    <row r="129" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A129" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B129" s="13"/>
+    </row>
+    <row r="130" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A130" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B130" s="13"/>
+    </row>
+    <row r="131" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A131" s="13"/>
+      <c r="B131" s="13"/>
+    </row>
+    <row r="132" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A132" s="13"/>
+      <c r="B132" s="13"/>
+    </row>
+    <row r="133" spans="1:2" ht="16" x14ac:dyDescent="0.8">
+      <c r="A133" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B120" s="13"/>
-    </row>
-    <row r="121" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B121" s="13"/>
-    </row>
-    <row r="122" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B122" s="13"/>
-    </row>
-    <row r="123" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="13"/>
-      <c r="B123" s="13"/>
-    </row>
-    <row r="124" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B124" s="13"/>
-    </row>
-    <row r="125" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="B125" s="13"/>
-    </row>
-    <row r="126" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A126" s="13"/>
-      <c r="B126" s="13"/>
-    </row>
-    <row r="127" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127" s="13"/>
-      <c r="B127" s="13"/>
-    </row>
-    <row r="128" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A128" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B128" s="13"/>
+      <c r="B133" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="A79:E79"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A84:E84"/>
+    <mergeCell ref="A85:E85"/>
     <mergeCell ref="A78:E78"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A25:E25"/>
@@ -2466,12 +2549,6 @@
     <mergeCell ref="A73:E73"/>
     <mergeCell ref="A74:E74"/>
     <mergeCell ref="A77:E77"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="A85:E85"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A104:C104">
@@ -2493,8 +2570,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A122" r:id="rId1" tooltip="https://www.banana.ch/apps/it/it/contabilita-terzo-settore/fino-a-300000" xr:uid="{A59A2887-F854-9A4D-8B4D-BE6E12243749}"/>
-    <hyperlink ref="A125" r:id="rId2" tooltip="https://www.banana.ch/it/node/9249" xr:uid="{B43AA590-682D-AE46-850F-5944AE67B430}"/>
+    <hyperlink ref="A127" r:id="rId1" tooltip="https://www.banana.ch/apps/it/it/contabilita-terzo-settore/fino-a-300000" xr:uid="{A59A2887-F854-9A4D-8B4D-BE6E12243749}"/>
+    <hyperlink ref="A130" r:id="rId2" tooltip="https://www.banana.ch/it/node/9249" xr:uid="{B43AA590-682D-AE46-850F-5944AE67B430}"/>
     <hyperlink ref="A115" r:id="rId3" xr:uid="{3790B8D1-CB6E-46EF-89B8-9A24475ADEDA}"/>
     <hyperlink ref="A116" r:id="rId4" xr:uid="{FAAD52DE-39AC-4ADB-93B1-F7F1CB7B8A23}"/>
   </hyperlinks>

</xml_diff>